<commit_message>
Colours applied for teams
</commit_message>
<xml_diff>
--- a/auction_data.xlsx
+++ b/auction_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seshu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seshu\Downloads\auction_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EFCDF9-6B54-429B-9903-148A8761B010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597AF687-F5E1-4EB0-9C80-38BF053B5F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E744E5E7-4E4D-4FA7-A329-0620FB9A679F}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Skill</t>
   </si>
@@ -62,24 +62,12 @@
     <t>Seshasai</t>
   </si>
   <si>
-    <t>All-rounder</t>
-  </si>
-  <si>
-    <t>Opening</t>
-  </si>
-  <si>
     <t>Vivek</t>
   </si>
   <si>
-    <t>Keeper-Batsman</t>
-  </si>
-  <si>
     <t>Deepak</t>
   </si>
   <si>
-    <t>Middle</t>
-  </si>
-  <si>
     <t>Budget</t>
   </si>
   <si>
@@ -87,6 +75,36 @@
   </si>
   <si>
     <t>Gagan</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>#FF7C7A</t>
+  </si>
+  <si>
+    <t>#7AD7FF</t>
+  </si>
+  <si>
+    <t>#FFEB7A</t>
+  </si>
+  <si>
+    <t>Right arm spin</t>
+  </si>
+  <si>
+    <t>Right Handed</t>
+  </si>
+  <si>
+    <t>Left Handed</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Right arm Medium</t>
+  </si>
+  <si>
+    <t>Right arm Medium Fast</t>
   </si>
 </sst>
 </file>
@@ -441,13 +459,14 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -469,10 +488,10 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>20</v>
@@ -480,13 +499,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -494,13 +513,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D4">
         <v>20</v>
@@ -508,13 +527,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>20</v>
@@ -528,56 +547,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CD7C14-CB86-411C-96E2-644406FE8558}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
         <v>500</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
         <v>500</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <v>500</v>
       </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated Players and Captains
</commit_message>
<xml_diff>
--- a/auction_data.xlsx
+++ b/auction_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seshu\Downloads\auction_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FD9695-6AD1-4A24-A050-06A2A1438C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE795AC-0E90-4BEA-8DD8-CA4854534455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E744E5E7-4E4D-4FA7-A329-0620FB9A679F}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
   <si>
     <t>Skill</t>
   </si>
@@ -59,21 +59,12 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Vivek</t>
-  </si>
-  <si>
-    <t>Deepak</t>
-  </si>
-  <si>
     <t>Budget</t>
   </si>
   <si>
     <t>Players</t>
   </si>
   <si>
-    <t>Gagan</t>
-  </si>
-  <si>
     <t>Color</t>
   </si>
   <si>
@@ -86,32 +77,137 @@
     <t>#FFEB7A</t>
   </si>
   <si>
-    <t>Right arm spin</t>
-  </si>
-  <si>
     <t>Right Handed</t>
   </si>
   <si>
     <t>Left Handed</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Right arm Medium</t>
-  </si>
-  <si>
-    <t>Right arm Medium Fast</t>
-  </si>
-  <si>
-    <t>Seshasai, Naishadham</t>
+    <t>Ravichandran, Harshini</t>
+  </si>
+  <si>
+    <t>Right Arm Throw (Ladies)</t>
+  </si>
+  <si>
+    <t>Dilip Toche, Pooja</t>
+  </si>
+  <si>
+    <t>Priyambada, Pallabi</t>
+  </si>
+  <si>
+    <t>Ashok Jujagar, Ankita</t>
+  </si>
+  <si>
+    <t>Dange, Shilpa</t>
+  </si>
+  <si>
+    <t>Rambhau Pachghare, Vishwas</t>
+  </si>
+  <si>
+    <t>Kujur, Animesh Aman</t>
+  </si>
+  <si>
+    <t>Basava, T Channa</t>
+  </si>
+  <si>
+    <t>Molabanti, Sai Manoj</t>
+  </si>
+  <si>
+    <t>Kumar, Sujith B</t>
+  </si>
+  <si>
+    <t>Krishna Chaithanya, Morla</t>
+  </si>
+  <si>
+    <t>Konga Reddy, Rajasekhar</t>
+  </si>
+  <si>
+    <t>Pavan, Kalyan</t>
+  </si>
+  <si>
+    <t>Singh Kapoor, Karandeep</t>
+  </si>
+  <si>
+    <t>Chowdhury Chirumamilla, Aravind</t>
+  </si>
+  <si>
+    <t>Kola, Satish</t>
+  </si>
+  <si>
+    <t>Kumar Mitra, Pranab</t>
+  </si>
+  <si>
+    <t>Narasimha Naishadham, Seshasai</t>
+  </si>
+  <si>
+    <t>Right Arm Spin</t>
+  </si>
+  <si>
+    <t>J C, Gagan Kumar</t>
+  </si>
+  <si>
+    <t>Right Arm Pace</t>
+  </si>
+  <si>
+    <t>K Muralidhar, Deepak</t>
+  </si>
+  <si>
+    <t>Kumar Gautam, Vivek</t>
+  </si>
+  <si>
+    <t>Verma, Rajeev</t>
+  </si>
+  <si>
+    <t>Raza, Mohammad</t>
+  </si>
+  <si>
+    <t>Manjrekar, Prathamesh</t>
+  </si>
+  <si>
+    <t>Agrawal, Aman</t>
+  </si>
+  <si>
+    <t>Babarao Panurkar, Prasad</t>
+  </si>
+  <si>
+    <t>Bhatia, Varsha Prakash</t>
+  </si>
+  <si>
+    <t>Fabio</t>
+  </si>
+  <si>
+    <t>Not Bowler</t>
+  </si>
+  <si>
+    <t>Rudy</t>
+  </si>
+  <si>
+    <t>Vilas Tonapi, Nitin</t>
+  </si>
+  <si>
+    <t>Avinash</t>
+  </si>
+  <si>
+    <t>Rupchand More, Amit</t>
+  </si>
+  <si>
+    <t>Kumar, Chandan (C)</t>
+  </si>
+  <si>
+    <t>Tripathy, Amrit (C)</t>
+  </si>
+  <si>
+    <t>Amalraj, Danny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mishra, Atulit Kumar (C) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,13 +215,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -140,13 +254,244 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -157,6 +502,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00C937D8-3935-4208-957F-8EA759955F94}" name="Table1" displayName="Table1" ref="A1:D37" totalsRowShown="0" dataDxfId="19">
+  <autoFilter ref="A1:D37" xr:uid="{00C937D8-3935-4208-957F-8EA759955F94}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D37">
+    <sortCondition sortBy="cellColor" ref="A2:A37" dxfId="3"/>
+    <sortCondition sortBy="cellColor" ref="A2:A37" dxfId="2"/>
+    <sortCondition ref="C2:C37"/>
+    <sortCondition ref="A2:A37"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{63918A9D-7CBD-4E60-8AE2-215D6BBBF624}" name="Player Name" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{8D96D033-2BEB-484C-BA5E-F6C7A7476803}" name="Skill" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{941294DC-BDEF-4D26-9389-AA254DE5134A}" name="Position" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{E5EE6B24-74AD-4790-8514-63B2FD498B09}" name="Base Price"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -456,17 +820,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6485261C-3E57-4A34-A6CE-984683E16939}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -484,64 +849,526 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5">
-        <v>200</v>
-      </c>
+      <c r="B36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D37">
+    <sortCondition sortBy="cellColor" ref="A2:A37" dxfId="21"/>
+    <sortCondition sortBy="cellColor" ref="A2:A37" dxfId="20"/>
+    <sortCondition ref="C2:C37"/>
+    <sortCondition ref="A2:A37"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -550,7 +1377,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,13 +1393,13 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -583,7 +1410,7 @@
         <v>10000</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -594,7 +1421,7 @@
         <v>10000</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -605,7 +1432,7 @@
         <v>10000</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>